<commit_message>
-Add Tvs diode -Update the LOGO -Fix the clearance and soldermask  layer issues
</commit_message>
<xml_diff>
--- a/Rleased/BOM/H3BR7.xlsx
+++ b/Rleased/BOM/H3BR7.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\HEXABITZ\Modules\Hardware\Modules Hardware Design\H3BR7x-Hardware\Rleased\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52E09477-0BF2-42CF-AFF2-0FC803D1BE99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3756C70-6A0E-4890-9BD2-FEA0CD338F84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="21840" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="H3BR7" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="102">
   <si>
     <t>Description</t>
   </si>
@@ -327,6 +327,21 @@
   </si>
   <si>
     <t xml:space="preserve">6-Digit 7-Segment Red Display Module (H3BR7) </t>
+  </si>
+  <si>
+    <t>D2</t>
+  </si>
+  <si>
+    <t>TVS DIODE 3,3V 10,9V SOD323</t>
+  </si>
+  <si>
+    <t>CDSOD323-T03SC</t>
+  </si>
+  <si>
+    <t>BOURNS INC</t>
+  </si>
+  <si>
+    <t>https://octopart.com/cdsod323-t03sc-bourns-10487153?r=sp</t>
   </si>
 </sst>
 </file>
@@ -525,7 +540,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -604,6 +619,18 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -980,10 +1007,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I25"/>
+  <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1322,101 +1349,101 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:6" s="16" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A20" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="B20" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="C20" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="D20" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="E20" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="F20" s="19">
-        <v>4</v>
+    <row r="20" spans="1:6" s="16" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A20" s="29" t="s">
+        <v>97</v>
+      </c>
+      <c r="B20" s="30" t="s">
+        <v>98</v>
+      </c>
+      <c r="C20" s="30" t="s">
+        <v>99</v>
+      </c>
+      <c r="D20" s="30" t="s">
+        <v>100</v>
+      </c>
+      <c r="E20" s="31" t="s">
+        <v>101</v>
+      </c>
+      <c r="F20" s="32">
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:6" s="16" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A21" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="B21" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="D21" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="E21" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="F21" s="19">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" s="16" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A22" s="17" t="s">
         <v>95</v>
       </c>
-      <c r="B21" s="17" t="s">
+      <c r="B22" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="C21" s="17" t="s">
+      <c r="C22" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="D21" s="17" t="s">
+      <c r="D22" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="E21" s="18" t="s">
+      <c r="E22" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="F21" s="19">
+      <c r="F22" s="19">
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:6" s="16" customFormat="1" ht="39.6" x14ac:dyDescent="0.25">
-      <c r="A22" s="17" t="s">
+    <row r="23" spans="1:6" s="16" customFormat="1" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A23" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="B22" s="17" t="s">
+      <c r="B23" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="C22" s="17" t="s">
+      <c r="C23" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="D22" s="17" t="s">
+      <c r="D23" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="E22" s="18" t="s">
+      <c r="E23" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="F22" s="19">
+      <c r="F23" s="19">
         <v>8</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="B23" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="C23" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="D23" s="17" t="s">
-        <v>92</v>
-      </c>
-      <c r="E23" s="18" t="s">
-        <v>82</v>
-      </c>
-      <c r="F23" s="19">
-        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:6" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="17" t="s">
-        <v>24</v>
+        <v>50</v>
       </c>
       <c r="B24" s="17" t="s">
-        <v>25</v>
+        <v>51</v>
       </c>
       <c r="C24" s="17" t="s">
-        <v>23</v>
+        <v>50</v>
       </c>
       <c r="D24" s="17" t="s">
-        <v>26</v>
+        <v>92</v>
       </c>
       <c r="E24" s="18" t="s">
-        <v>27</v>
+        <v>82</v>
       </c>
       <c r="F24" s="19">
         <v>1</v>
@@ -1424,21 +1451,41 @@
     </row>
     <row r="25" spans="1:6" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="B25" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="C25" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="D25" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="E25" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="F25" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="B25" s="17" t="s">
+      <c r="B26" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="C25" s="17" t="s">
+      <c r="C26" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="D25" s="17" t="s">
+      <c r="D26" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="E25" s="18" t="s">
+      <c r="E26" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="F25" s="19">
+      <c r="F26" s="19">
         <v>1</v>
       </c>
     </row>
@@ -1451,17 +1498,17 @@
   <hyperlinks>
     <hyperlink ref="C19" r:id="rId1" display="https://octopart.com/manufacturers/wolfspeed" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
     <hyperlink ref="E12" r:id="rId2" display="https://octopart.com/cl05a106mp8nub8-samsung-68086897?r=sp" xr:uid="{1CA08D75-7CE2-4798-BFB4-4DFC1825B006}"/>
-    <hyperlink ref="E20" r:id="rId3" display="https://octopart.com/87227-1-te+connectivity-39512052?r=sp" xr:uid="{97DC24F0-08CA-4316-A0CB-F81F9DEADBAB}"/>
+    <hyperlink ref="E21" r:id="rId3" display="https://octopart.com/87227-1-te+connectivity-39512052?r=sp" xr:uid="{97DC24F0-08CA-4316-A0CB-F81F9DEADBAB}"/>
     <hyperlink ref="E18" r:id="rId4" display="https://octopart.com/search?q=RC0603FR-0710KL&amp;currency=USD&amp;specs=0" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="E23" r:id="rId5" display="https://octopart.com/search?q=060300F2201T5E&amp;currency=USD&amp;specs=0" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="E24" r:id="rId5" display="https://octopart.com/search?q=060300F2201T5E&amp;currency=USD&amp;specs=0" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
     <hyperlink ref="E14" r:id="rId6" display="https://octopart.com/erj-3geyj271v-panasonic-55560546" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
     <hyperlink ref="E11" r:id="rId7" display="https://octopart.com/10tpu4r7msi-panasonic-29487748?r=sp" xr:uid="{23CC8D52-00B7-424D-AE6F-D90CF0F8A6D7}"/>
     <hyperlink ref="E16" r:id="rId8" xr:uid="{636BB640-56DA-4B3A-8EBB-00A74F7EF75D}"/>
     <hyperlink ref="E10" r:id="rId9" display="https://octopart.com/c0603c104k8ractu-kemet-145075?r=sp&amp;s=9bS9ASSwSEqMCE9KBEQZ0g" xr:uid="{663B604C-0778-4D31-8D01-1E3B83AE8D9B}"/>
     <hyperlink ref="E13" r:id="rId10" display="https://octopart.com/rc0603jr-070rl-yageo-1241539?r=sp" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
     <hyperlink ref="E19" r:id="rId11" display="https://octopart.com/vlms1300-gs08-vishay-21709201?r=sp&amp;s=_gcP4_q8T1SC6PJQPTQ9yA" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="E24" r:id="rId12" display="https://octopart.com/search?q=MPZ1608S601ATD25&amp;currency=USD&amp;specs=0" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="E25" r:id="rId13" display="https://octopart.com/stm32g0b1ceu6n-stmicroelectronics-116364672?r=sp" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="E25" r:id="rId12" display="https://octopart.com/search?q=MPZ1608S601ATD25&amp;currency=USD&amp;specs=0" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="E26" r:id="rId13" display="https://octopart.com/stm32g0b1ceu6n-stmicroelectronics-116364672?r=sp" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId14"/>

</xml_diff>